<commit_message>
Connexion avec la base de données locale de l'utilisateur établie.
</commit_message>
<xml_diff>
--- a/Devis.xlsx
+++ b/Devis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PFE_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46DA23F4-F431-42B4-9463-923B06B53857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C476A9-25F0-4219-9F39-4AC8BF123943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{866B7D95-A557-4FB8-89D9-CA0A2A3AEFD9}"/>
   </bookViews>
@@ -18,23 +18,28 @@
   <definedNames>
     <definedName name="_Hlk127815411" localSheetId="0">Feuil1!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Quantite</t>
-  </si>
-  <si>
-    <t>Designation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Prix Unitaire (F CFA)</t>
   </si>
@@ -45,26 +50,74 @@
     <t>Ecran tactile 7’’ pour Raspberry pi</t>
   </si>
   <si>
-    <t>Module GPS</t>
-  </si>
-  <si>
-    <t>Batterie d'alimentation LiPo 12V</t>
-  </si>
-  <si>
-    <t>Chargeur de batterie LiPo</t>
-  </si>
-  <si>
-    <t>Carte Raspberry Pi 4</t>
-  </si>
-  <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Module Skywire GPS</t>
+  </si>
+  <si>
+    <t>Module Adafruit Ultimate GPS Breakout</t>
+  </si>
+  <si>
+    <t>Micro AMS 24189C PIR</t>
+  </si>
+  <si>
+    <t>Micro MEMS I2S PMB 404</t>
+  </si>
+  <si>
+    <t>Haut-parleur I2S PAM 8403</t>
+  </si>
+  <si>
+    <t>Haut-parleur USB PAM 8610</t>
+  </si>
+  <si>
+    <t>Antenne GPS Enduro Active RG 174 SMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenne GPS Passive DPCAV </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carte Raspberry Pi 4 supportant le mode </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>"adhoc"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Carte Raspberry Pi 3B+  supportant le mode</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> "adhoc"</t>
+    </r>
+  </si>
+  <si>
+    <t>Désignation</t>
+  </si>
+  <si>
+    <t>Quantité</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +125,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,15 +181,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60 % - Accent2" xfId="1" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -111,6 +233,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle : avec coins arrondis en diagonale 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C61D515D-D5BA-3465-49D6-A4F826A40715}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2219325" y="209549"/>
+          <a:ext cx="3228975" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="round2DiagRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="2000" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>DEVIS DU MATERIEL</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,127 +601,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0FF884-4506-4633-8C28-A6CB3895D95C}">
-  <dimension ref="B6:E12"/>
+  <dimension ref="B3:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="3" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <f>D7*B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <f t="shared" ref="E8:E17" si="0">D8*B8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>35000</v>
-      </c>
-      <c r="E7">
-        <f>D7*B7</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>65000</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8:E11" si="0">D8*B8</f>
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>5000</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>12000</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>5000</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12">
-        <f>SUM(D7:D11)</f>
-        <v>122000</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E7:E11)</f>
-        <v>122000</v>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4">
+        <f>SUM(D7:D17)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <f>SUM(E7:E17)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>